<commit_message>
Update data package at: 2024-01-23T23:39:47Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_base_legal_demonstrativos.xlsx
+++ b/data-raw/desc_base_legal_demonstrativos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\2.Programação e Normas\2023\PPAG 2023 e LOA 2023\Volumes\Demonstrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C42A1CD-4EA3-4A8C-A0B5-E81FF3644D5C}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0109EFDD-06D7-4D09-B34D-15123BD54272}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,8 +210,8 @@
     <t>25. Demonstrativo da Aplicação dos Recursos do Fundo de Desenvolvimento da Educação Básica e Valorização dos Profissionais da Educação</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
-da Lei 24.218/2022 - LDO)</t>
+    <t>(Art. 212-A da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
+da Lei 24.404/2023 - LDO)</t>
   </si>
   <si>
     <t>T26_DCGF_DEMONSTRATIVO_RECURSOS_APLICADOS_ACOES_PARA_CRIANCA_E_ADOLESCENTE</t>
@@ -832,7 +832,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1655,8 +1655,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c170a06b81d8b923cbfe6a63de8ee1c9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="844dfdedaab7989660d9d802f918fcda" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
     <xsd:import namespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
     <xsd:element name="properties">
@@ -1681,6 +1681,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1760,6 +1761,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1904,15 +1910,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
@@ -1931,14 +1928,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BBCCE74-F276-4B9C-8C51-FA44D9D6D69C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C048F50-7DE2-4464-BD5C-A1BECFD191AF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF4EF5B-0E3B-4873-A6D2-6087C9EC9166}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FCAB9D5-4699-48C8-8DB7-84FDCD7CDA0C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FCAB9D5-4699-48C8-8DB7-84FDCD7CDA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF4EF5B-0E3B-4873-A6D2-6087C9EC9166}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2024-09-25T16:51:50Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_base_legal_demonstrativos.xlsx
+++ b/data-raw/desc_base_legal_demonstrativos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\2.Programação e Normas\2023\PPAG 2023 e LOA 2023\Volumes\Demonstrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0109EFDD-06D7-4D09-B34D-15123BD54272}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38012AAB-ADD5-4129-895E-60B6F719184B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
   <si>
     <t>cod</t>
   </si>
@@ -57,7 +57,7 @@
     <t>02. Demonstrativo da Receita Corrente Fiscal</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XXII da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T3_DCGF_Demonstrativo_Receita_Despesa_Segundo_Categorias_Economicas</t>
@@ -84,7 +84,7 @@
     <t>05. Demonstrativo Consolidado da Categoria de Pessoal por Unidade Orçamentária</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXIII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XXIII da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T6_DCGF_Demonstrativo_Evolucao_Receita_por_Categoria_Economica</t>
@@ -111,7 +111,7 @@
     <t>08. Demonstrativo da Receita Corrente Líquida</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso II da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso II da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T9_DEMONSTRATIVO_RECEITA_ORCAMENTARIA_CORRENTE_ORDINARIA</t>
@@ -120,7 +120,7 @@
     <t>09. Demonstrativo da Receita Orçamentária Corrente Ordinária</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XV da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XV da Lei 24.945/2024 -  LDO)</t>
   </si>
   <si>
     <t>T12_DCGF_Demonstrativo_Evolucao_Despesa_Categoria_Economica</t>
@@ -156,7 +156,7 @@
     <t>16. Demonstrativo da Aplicação de Recursos na Manutenção e no Desenvolvimento do Ensino</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Federal, Art. 201 da Constituição Estadual e Art. 7º, Inciso III da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 212 da Constituição Federal, Art. 201 da Constituição Estadual e Art. 7º, Inciso III da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T17_DCGF_Demonst_Aplicacao_Recursos_Progr_Saude_Investim</t>
@@ -165,7 +165,7 @@
     <t>17. Demonstrativo da Aplicação de Recursos em Programas de Saúde e em Investimentos em Transporte e Sistema Viário</t>
   </si>
   <si>
-    <t>(Art. 158 da Constituição Estadual e Art. 7º, Inciso IV da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 158,  §1º da Constituição Estadual e Art. 7º, Inciso IV da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T18_DCGF_Demonst_Aplicacao_Recursos_Acoes_Servicos_Publicos_Saude</t>
@@ -174,7 +174,7 @@
     <t>18. Demonstrativo da Aplicação de Recursos em Ações e Serviços Públicos de Saúde</t>
   </si>
   <si>
-    <t>(Art. 198 da Constituição Federal e Art. 7°, Inciso V da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 198 da Constituição Federal e Art. 7°, Inciso V da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T19_DCGF_Demonstrativo_Aplicacao_Recursos_Amparo_Fomento_Pesquisa</t>
@@ -183,7 +183,7 @@
     <t>19. Demonstrativo da Aplicação de Recursos no Amparo e Fomento à Pesquisa</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Estadual e Art. 7°, Inciso VI da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 212 da Constituição Estadual e Art. 7°, Inciso VI da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T20A_DCGF_Demonstrativo_Partic_Percentual_Pessoal_RCL_LRF</t>
@@ -192,7 +192,7 @@
     <t>20. Demonstrativo da Participação Percentual de Pessoal na Receita Corrente Líquida</t>
   </si>
   <si>
-    <t>(Art. 19 da Lei Complementar 101/2000 - LRF e Art. 7°, Inciso VIII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 19 da Lei Complementar 101/2000 - LRF e Art. 7°, Inciso VIII da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T23_DCGF_Demonstrativo_do_Servico_da_divida_publica</t>
@@ -201,7 +201,7 @@
     <t>23. Demonstrativo do Serviço da Dívida Pública</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XIII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XIII da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T25_DCGF_Demonstrativo_Aplicacao_Recursos_FUNDEB</t>
@@ -210,8 +210,8 @@
     <t>25. Demonstrativo da Aplicação dos Recursos do Fundo de Desenvolvimento da Educação Básica e Valorização dos Profissionais da Educação</t>
   </si>
   <si>
-    <t>(Art. 212-A da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
-da Lei 24.404/2023 - LDO)</t>
+    <t xml:space="preserve">(Art. 212-A da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
+da Lei 24.945/2024 - LDO)                                                                                                                                               </t>
   </si>
   <si>
     <t>T26_DCGF_DEMONSTRATIVO_RECURSOS_APLICADOS_ACOES_PARA_CRIANCA_E_ADOLESCENTE</t>
@@ -220,7 +220,7 @@
     <t>26.  Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, em ações voltadas para a criança e o adolescente</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XVIII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XVIII da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T27_DCGF_Demonst_Despesas_UGEPREVI</t>
@@ -229,7 +229,7 @@
     <t>27. Demonstrativo  das  despesas  da  Unidade  de  Gestão Previdenciária  Integrada  -  UGEPREVI</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso X da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso X da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T38_DCGF_DEMONSTRATIVO_RECEITAS_DESPESAS_PREVIDENCIARIAS_RPPS</t>
@@ -238,7 +238,7 @@
     <t>28. Demonstrativo das Receitas e Despesas Previdenciárias</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XI da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XI da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T28_DCGF</t>
@@ -247,7 +247,7 @@
     <t>29. Demonstrativo dos programas financiados com recursos provenientes da União</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XX da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XX da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T30_INVESTIMENTOS_SEGUNDO_FUNCOES</t>
@@ -256,7 +256,7 @@
     <t>32. Investimentos Segundo as Funções</t>
   </si>
   <si>
-    <t>(Art. 2º, §1º, Inciso I da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 2°, §1°, Inciso I da Lei 4.320/64)</t>
   </si>
   <si>
     <t>T31_INVESTIMENTOS_SEGUNDO_FUNCOES_SUBFUNCOES_PROGRAMAS_POR_PROJETOS_ATIVIDADES</t>
@@ -265,7 +265,7 @@
     <t>33. Investimentos Segundo Funções, Subfunções e Programas por Projetos e Atividades</t>
   </si>
   <si>
-    <t>(Art. 32 da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 31 da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>T32_INVESTIMENTOS_POR_EMPRESA_SEGUNDO_FONTES_RECURSO</t>
@@ -274,6 +274,9 @@
     <t>34. Investimentos por Empresas Segundo Fonte de Recurso</t>
   </si>
   <si>
+    <t>(Art. 32 da Lei 24.945/2024 - LDO)</t>
+  </si>
+  <si>
     <t>T33_INVESTIMENTOS_EMPRESA_SEGUNDO_DETALHAMENTO_INVESTIMENTOS</t>
   </si>
   <si>
@@ -286,7 +289,16 @@
     <t>38.    Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na  execução  da  Política  Estadual  de Segurança Alimentar e Nutricional Sustentável - PESANS</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XVII da Lei 24.404/2023 - LDO)</t>
+    <t>(Art. 7º, Inciso XVII da Lei 24.945/2024 - LDO)</t>
+  </si>
+  <si>
+    <t>T39_DCGF_DEMONSTRATIVO_DA_POLITICA_DE_ATENDIMENTO_A_MULHER_VITIMA_DE_VIOLENCIA_NO_ESTADO</t>
+  </si>
+  <si>
+    <t>41. Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na execução da política de atendimento à mulher vítima de violência no Estado, conforme o disposto na Lei nº 22.256, de 26 de julho de 2016.</t>
+  </si>
+  <si>
+    <t>(Art. 7º, Inciso XXV da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>DEMONSTRATIVOS CONSOLIDADOS DO ORÇAMENTO FISCAL</t>
@@ -316,98 +328,46 @@
     <t>01. Demonstrativo Consolidado do Orçamento Fiscal</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso I da Lei 24.404/2023- LDO)</t>
+    <t>(Art. 7º, Inciso I da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXII da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XXIII da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso II da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XV da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
     <t>10. Demonstrativo da Previsão de Arrecadação do ICMS Discriminado por Gênero</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XIV da Lei 24.404/2023- LDO)</t>
+    <t>(Art. 7º, Inciso XIV da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>11. Legislação da Receita</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Federal, Art. 201 da Constituição Estadual e Art. 7º, Inciso III da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 158 da Constituição Estadual e Art. 7º, Inciso IV da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 198 da Constituição Federal e Art. 7°, Inciso V da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 212 da Constituição Estadual e Art. 7°, Inciso VI da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 19 da Lei Complementar 101/2000 - LRF e Art. 7°, Inciso VIII da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
     <t>21. Demonstrativo Regionalizado do Efeito sobre a Receita e a Despesa Decorrente de Benefícios Fiscais</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso IX da Lei Lei 24.404/2023- LDO)</t>
+    <t>(Art. 7º, Inciso IX da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>22. Demonstrativo Regionalizado, em Valores Nominais e Percentuais, das Despesas Decorrentes de Atividade de Fomento do Estado, por Função Orçamentária e Tipo de Receita (A e B)</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XVI da Lei Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XIII da Lei Lei 24.404/2023- LDO)</t>
+    <t>(Art. 7º, Inciso XVI da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t xml:space="preserve">24. Memória de Cálculo e Quadro Detalhado do Serviço da Dívida </t>
   </si>
   <si>
-    <t xml:space="preserve">(Art. 212 da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
-da Lei 24.218/2022 - LDO)                                                                                                                                                            </t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XVIII da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso X da Lei Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XI da Lei Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XX da Lei Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
     <t xml:space="preserve">30. Demonstrativo Regionalizado do Orçamento Fiscal, em valores nominais, a ser aplicado por função </t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXI da Lei Lei 24.404/2023- LDO)</t>
+    <t>(Art. 7º, Inciso XXI da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>31. Demonstrativo Transferências Voluntárias</t>
   </si>
   <si>
-    <t>(Art. 24 da Lei Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 2º, §1º, Inciso I da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 32 da Lei 24.404/2023- LDO)</t>
+    <t>(Art. 24 da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t xml:space="preserve">36. Composição da Participação Societária no Capital das Empresas </t>
@@ -416,29 +376,26 @@
     <t>37.    PLANO DE APLICAÇÃO DOS RECURSOS DO BDMG E DOS FUNDOS ESTADUAIS</t>
   </si>
   <si>
-    <t>(Art. 58 da Lei 24.404/2023- LDO)</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XVII da Lei 24.404/2023- LDO</t>
+    <t>(Art. 57 da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>39. Demonstrativo dos recursos a serem aplicados no desenvolvimento social dos municípios classificados nas cinquenta últimas posições no relatório do Índice Mineiro de Responsabilidade Social - IMRS</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XIX da Lei 24.404/2023- LDO</t>
+    <t>(Art. 7º, Inciso XIX da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>40.    GRUPOS DE DESPESA, FONTES DE RECURSO, IDENTIFICADORES DE PROCEDÊNCIA E USO E IDENTIFICADORES DE AÇÃO GOVERNAMENTAL</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXIV da Lei 24.404/2023- LDO</t>
+    <t>(Art. 7º, Inciso XXIV da Lei 24.945/2024 - LDO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,8 +433,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +458,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -520,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -547,6 +517,9 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -829,17 +802,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="167.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="197.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="116" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1051,14 +1025,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30.75">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1136,29 +1110,40 @@
         <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1169,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9730DD9-C36A-40E7-998B-E00A0695F1C5}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1184,39 +1169,39 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30.75">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30.75">
@@ -1224,10 +1209,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30.75">
@@ -1238,7 +1223,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30.75">
@@ -1249,7 +1234,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30.75">
@@ -1257,10 +1242,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1271,7 +1256,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30.75">
@@ -1282,7 +1267,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30.75">
@@ -1290,10 +1275,10 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30.75">
@@ -1301,10 +1286,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30.75">
@@ -1315,7 +1300,7 @@
         <v>98</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30.75">
@@ -1326,7 +1311,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1337,7 +1322,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30.75">
@@ -1348,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30.75">
@@ -1359,7 +1344,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30.75">
@@ -1370,7 +1355,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60.75">
@@ -1378,10 +1363,10 @@
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45.75">
@@ -1389,10 +1374,10 @@
         <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45.75">
@@ -1400,10 +1385,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45.75">
@@ -1411,10 +1396,10 @@
         <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45.75">
@@ -1422,32 +1407,32 @@
         <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30.75">
       <c r="A22" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="37.5">
       <c r="A23" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30.75">
@@ -1455,21 +1440,21 @@
         <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30.75">
       <c r="A25" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="60.75">
@@ -1477,10 +1462,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30.75">
@@ -1488,10 +1473,10 @@
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -1500,10 +1485,10 @@
         <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30.75">
@@ -1511,10 +1496,10 @@
         <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30.75">
@@ -1522,43 +1507,43 @@
         <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30.75">
       <c r="A31" s="8" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="8" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30.75">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1566,10 +1551,10 @@
         <v>73</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1577,76 +1562,87 @@
         <v>76</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="8" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="8" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30.75">
       <c r="A39" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="37.5">
       <c r="A40" s="8" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30.75">
       <c r="A41" s="8" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="34.5" customHeight="1">
+      <c r="A42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1655,6 +1651,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -1909,36 +1933,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C048F50-7DE2-4464-BD5C-A1BECFD191AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF4EF5B-0E3B-4873-A6D2-6087C9EC9166}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1946,5 +1942,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF4EF5B-0E3B-4873-A6D2-6087C9EC9166}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C048F50-7DE2-4464-BD5C-A1BECFD191AF}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2024-09-25T19:27:55Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_base_legal_demonstrativos.xlsx
+++ b/data-raw/desc_base_legal_demonstrativos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\2.Programação e Normas\2023\PPAG 2023 e LOA 2023\Volumes\Demonstrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38012AAB-ADD5-4129-895E-60B6F719184B}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C08B51-1281-4B62-B67B-460FE125EE8F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_legal" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
     <t>T30_INVESTIMENTOS_SEGUNDO_FUNCOES</t>
   </si>
   <si>
-    <t>32. Investimentos Segundo as Funções</t>
+    <t>33. Investimentos Segundo as Funções</t>
   </si>
   <si>
     <t>(Art. 2°, §1°, Inciso I da Lei 4.320/64)</t>
@@ -262,7 +262,7 @@
     <t>T31_INVESTIMENTOS_SEGUNDO_FUNCOES_SUBFUNCOES_PROGRAMAS_POR_PROJETOS_ATIVIDADES</t>
   </si>
   <si>
-    <t>33. Investimentos Segundo Funções, Subfunções e Programas por Projetos e Atividades</t>
+    <t>34. Investimentos Segundo Funções, Subfunções e Programas por Projetos e Atividades</t>
   </si>
   <si>
     <t>(Art. 31 da Lei 24.945/2024 - LDO)</t>
@@ -271,7 +271,7 @@
     <t>T32_INVESTIMENTOS_POR_EMPRESA_SEGUNDO_FONTES_RECURSO</t>
   </si>
   <si>
-    <t>34. Investimentos por Empresas Segundo Fonte de Recurso</t>
+    <t>35. Investimentos por Empresas Segundo Fonte de Recurso</t>
   </si>
   <si>
     <t>(Art. 32 da Lei 24.945/2024 - LDO)</t>
@@ -280,13 +280,13 @@
     <t>T33_INVESTIMENTOS_EMPRESA_SEGUNDO_DETALHAMENTO_INVESTIMENTOS</t>
   </si>
   <si>
-    <t>35. Investimentos por Empresas Segundo o Detalhamento dos Investimentos</t>
+    <t>36. Investimentos por Empresas Segundo o Detalhamento dos Investimentos</t>
   </si>
   <si>
     <t>T37_DCGF_DEMONSTRATIVOS_RECURSOS_APLICADOS_SEGURANCA_ALIMENTAR_NUTRICIONAL</t>
   </si>
   <si>
-    <t>38.    Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na  execução  da  Política  Estadual  de Segurança Alimentar e Nutricional Sustentável - PESANS</t>
+    <t>39.    Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na  execução  da  Política  Estadual  de Segurança Alimentar e Nutricional Sustentável - PESANS</t>
   </si>
   <si>
     <t>(Art. 7º, Inciso XVII da Lei 24.945/2024 - LDO)</t>
@@ -295,7 +295,7 @@
     <t>T39_DCGF_DEMONSTRATIVO_DA_POLITICA_DE_ATENDIMENTO_A_MULHER_VITIMA_DE_VIOLENCIA_NO_ESTADO</t>
   </si>
   <si>
-    <t>41. Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na execução da política de atendimento à mulher vítima de violência no Estado, conforme o disposto na Lei nº 22.256, de 26 de julho de 2016.</t>
+    <t>34. Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na execução da política de atendimento à mulher vítima de violência no Estado, conforme o disposto na Lei nº 22.256, de 26 de julho de 2016.</t>
   </si>
   <si>
     <t>(Art. 7º, Inciso XXV da Lei 24.945/2024 - LDO)</t>
@@ -370,22 +370,22 @@
     <t>(Art. 24 da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
-    <t xml:space="preserve">36. Composição da Participação Societária no Capital das Empresas </t>
-  </si>
-  <si>
-    <t>37.    PLANO DE APLICAÇÃO DOS RECURSOS DO BDMG E DOS FUNDOS ESTADUAIS</t>
+    <t xml:space="preserve">37. Composição da Participação Societária no Capital das Empresas </t>
+  </si>
+  <si>
+    <t>38.    PLANO DE APLICAÇÃO DOS RECURSOS DO BDMG E DOS FUNDOS ESTADUAIS</t>
   </si>
   <si>
     <t>(Art. 57 da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
-    <t>39. Demonstrativo dos recursos a serem aplicados no desenvolvimento social dos municípios classificados nas cinquenta últimas posições no relatório do Índice Mineiro de Responsabilidade Social - IMRS</t>
+    <t>40. Demonstrativo dos recursos a serem aplicados no desenvolvimento social dos municípios classificados nas cinquenta últimas posições no relatório do Índice Mineiro de Responsabilidade Social - IMRS</t>
   </si>
   <si>
     <t>(Art. 7º, Inciso XIX da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
-    <t>40.    GRUPOS DE DESPESA, FONTES DE RECURSO, IDENTIFICADORES DE PROCEDÊNCIA E USO E IDENTIFICADORES DE AÇÃO GOVERNAMENTAL</t>
+    <t>41.    GRUPOS DE DESPESA, FONTES DE RECURSO, IDENTIFICADORES DE PROCEDÊNCIA E USO E IDENTIFICADORES DE AÇÃO GOVERNAMENTAL</t>
   </si>
   <si>
     <t>(Art. 7º, Inciso XXIV da Lei 24.945/2024 - LDO)</t>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9730DD9-C36A-40E7-998B-E00A0695F1C5}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1535,12 +1535,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>71</v>
+    <row r="33" spans="1:6" ht="40.5" customHeight="1">
+      <c r="A33" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>96</v>
@@ -1548,10 +1548,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>96</v>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>96</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>77</v>
@@ -1580,68 +1580,68 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="8" t="s">
-        <v>109</v>
+      <c r="A37" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30.75">
-      <c r="A39" s="2" t="s">
+      <c r="F39" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30.75">
+      <c r="A40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="37.5">
-      <c r="A40" s="8" t="s">
+      <c r="C40" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="37.5">
+      <c r="A41" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30.75">
-      <c r="A41" s="8" t="s">
+      <c r="D41" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30.75">
+      <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A42" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1660,25 +1660,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -1933,14 +1914,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF4EF5B-0E3B-4873-A6D2-6087C9EC9166}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FCAB9D5-4699-48C8-8DB7-84FDCD7CDA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C048F50-7DE2-4464-BD5C-A1BECFD191AF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C048F50-7DE2-4464-BD5C-A1BECFD191AF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FCAB9D5-4699-48C8-8DB7-84FDCD7CDA0C}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2025-09-27T01:39:51Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_base_legal_demonstrativos.xlsx
+++ b/data-raw/desc_base_legal_demonstrativos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecad365.sharepoint.com/sites/Splor/Documentos Compartilhados/General/@dcppn/DCPPN 2026/PPAG e LOA 2026/PPAG/material de apoio - gerar volumes/2026/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecad365.sharepoint.com/sites/Splor/Documentos Compartilhados/General/@dcppn/DCPPN 2026/PPAG e LOA 2026/material de apoio/material de apoio - gerar volumes/2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8601CC6-C21C-4811-ABA2-F524E54DC065}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="11_A3DD8646BA7476893AAB1FDD9F017BEA3498940F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AABACC1-D64D-48C7-8AD2-BF49F9BB0DE6}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_legal" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="136">
   <si>
     <t>cod</t>
   </si>
@@ -60,9 +60,6 @@
     <t>02. Demonstrativo da Receita Corrente Fiscal</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T3_DCGF_Demonstrativo_Receita_Despesa_Segundo_Categorias_Economicas</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>05. Demonstrativo Consolidado da Categoria de Pessoal por Unidade Orçamentária</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XXIII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T6_DCGF_Demonstrativo_Evolucao_Receita_por_Categoria_Economica</t>
   </si>
   <si>
@@ -114,18 +108,12 @@
     <t>08. Demonstrativo da Receita Corrente Líquida</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso II da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T9_DEMONSTRATIVO_RECEITA_ORCAMENTARIA_CORRENTE_ORDINARIA</t>
   </si>
   <si>
     <t>09. Demonstrativo da Receita Orçamentária Corrente Ordinária</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XV da Lei 24.945/2024 -  LDO)</t>
-  </si>
-  <si>
     <t>T12_DCGF_Demonstrativo_Evolucao_Despesa_Categoria_Economica</t>
   </si>
   <si>
@@ -159,100 +147,66 @@
     <t>16. Demonstrativo da Aplicação de Recursos na Manutenção e no Desenvolvimento do Ensino</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Federal, Art. 201 da Constituição Estadual e Art. 7º, Inciso III da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T17_DCGF_Demonst_Aplicacao_Recursos_Progr_Saude_Investim</t>
   </si>
   <si>
     <t>17. Demonstrativo da Aplicação de Recursos em Programas de Saúde e em Investimentos em Transporte e Sistema Viário</t>
   </si>
   <si>
-    <t>(Art. 158,  §1º da Constituição Estadual e Art. 7º, Inciso IV da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T18_DCGF_Demonst_Aplicacao_Recursos_Acoes_Servicos_Publicos_Saude</t>
   </si>
   <si>
     <t>18. Demonstrativo da Aplicação de Recursos em Ações e Serviços Públicos de Saúde</t>
   </si>
   <si>
-    <t>(Art. 198 da Constituição Federal e Art. 7°, Inciso V da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T19_DCGF_Demonstrativo_Aplicacao_Recursos_Amparo_Fomento_Pesquisa</t>
   </si>
   <si>
     <t>19. Demonstrativo da Aplicação de Recursos no Amparo e Fomento à Pesquisa</t>
   </si>
   <si>
-    <t>(Art. 212 da Constituição Estadual e Art. 7°, Inciso VI da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T20A_DCGF_Demonstrativo_Partic_Percentual_Pessoal_RCL_LRF</t>
   </si>
   <si>
     <t>20. Demonstrativo da Participação Percentual de Pessoal na Receita Corrente Líquida</t>
   </si>
   <si>
-    <t>(Art. 19 da Lei Complementar 101/2000 - LRF e Art. 7°, Inciso VIII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T23_DCGF_Demonstrativo_do_Servico_da_divida_publica</t>
   </si>
   <si>
     <t>23. Demonstrativo do Serviço da Dívida Pública</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XIII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T25_DCGF_Demonstrativo_Aplicacao_Recursos_FUNDEB</t>
   </si>
   <si>
     <t>25. Demonstrativo da Aplicação dos Recursos do Fundo de Desenvolvimento da Educação Básica e Valorização dos Profissionais da Educação</t>
   </si>
   <si>
-    <t xml:space="preserve">(Art. 212-A da Constituição Federal, Art. 60 do ADCT/CF e Art. 7°, Inciso XII
-da Lei 24.945/2024 - LDO)                                                                                                                                               </t>
-  </si>
-  <si>
     <t>T26_DCGF_DEMONSTRATIVO_RECURSOS_APLICADOS_ACOES_PARA_CRIANCA_E_ADOLESCENTE</t>
   </si>
   <si>
     <t>26.  Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, em ações voltadas para a criança e o adolescente</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XVIII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T27_DCGF_Demonst_Despesas_UGEPREVI</t>
   </si>
   <si>
     <t>27. Demonstrativo  das  despesas  da  Unidade  de  Gestão Previdenciária  Integrada  -  UGEPREVI</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso X da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T38_DCGF_DEMONSTRATIVO_RECEITAS_DESPESAS_PREVIDENCIARIAS_RPPS</t>
   </si>
   <si>
     <t>28. Demonstrativo das Receitas e Despesas Previdenciárias</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XI da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T28_DCGF</t>
   </si>
   <si>
     <t>29. Demonstrativo dos programas financiados com recursos provenientes da União</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XX da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T30_INVESTIMENTOS_SEGUNDO_FUNCOES</t>
   </si>
   <si>
@@ -268,18 +222,12 @@
     <t>34. Investimentos Segundo Funções, Subfunções e Programas por Projetos e Atividades</t>
   </si>
   <si>
-    <t>(Art. 31 da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T32_INVESTIMENTOS_POR_EMPRESA_SEGUNDO_FONTES_RECURSO</t>
   </si>
   <si>
     <t>35. Investimentos por Empresas Segundo Fonte de Recurso</t>
   </si>
   <si>
-    <t>(Art. 32 da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T33_INVESTIMENTOS_EMPRESA_SEGUNDO_DETALHAMENTO_INVESTIMENTOS</t>
   </si>
   <si>
@@ -292,16 +240,10 @@
     <t>39.    Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na  execução  da  Política  Estadual  de Segurança Alimentar e Nutricional Sustentável - PESANS</t>
   </si>
   <si>
-    <t>(Art. 7º, Inciso XVII da Lei 24.945/2024 - LDO)</t>
-  </si>
-  <si>
     <t>T39_DCGF_DEMONSTRATIVO_DA_POLITICA_DE_ATENDIMENTO_A_MULHER_VITIMA_DE_VIOLENCIA_NO_ESTADO</t>
   </si>
   <si>
     <t>34. Demonstrativo dos recursos a serem aplicados, direta ou indiretamente, na execução da política de atendimento à mulher vítima de violência no Estado, conforme o disposto na Lei nº 22.256, de 26 de julho de 2016.</t>
-  </si>
-  <si>
-    <t>(Art. 7º, Inciso XXV da Lei 24.945/2024 - LDO)</t>
   </si>
   <si>
     <t>DEMONSTRATIVOS CONSOLIDADOS DO ORÇAMENTO FISCAL</t>
@@ -1057,6 +999,7 @@
           <cell r="C27" t="str">
             <v>x</v>
           </cell>
+          <cell r="D27"/>
           <cell r="I27" t="str">
             <v>carolina</v>
           </cell>
@@ -1141,6 +1084,7 @@
           <cell r="C33" t="str">
             <v>x</v>
           </cell>
+          <cell r="D33"/>
           <cell r="I33" t="str">
             <v>Izabella</v>
           </cell>
@@ -1582,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,315 +1557,315 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1934,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9730DD9-C36A-40E7-998B-E00A0695F1C5}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,48 +1894,48 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="K1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I2" t="str">
         <f>VLOOKUP(A2,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2003,10 +1947,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I3" t="str">
         <f>VLOOKUP(A3,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2015,13 +1959,13 @@
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I4" t="str">
         <f>VLOOKUP(A4,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2030,41 +1974,41 @@
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I7" t="str">
         <f>VLOOKUP(A7,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2073,13 +2017,13 @@
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I8" t="str">
         <f>VLOOKUP(A8,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2088,13 +2032,13 @@
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I9" t="str">
         <f>VLOOKUP(A9,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2103,13 +2047,13 @@
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I10" t="str">
         <f>VLOOKUP(A10,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2118,13 +2062,13 @@
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I11" t="str">
         <f>VLOOKUP(A11,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2133,13 +2077,13 @@
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I12" t="str">
         <f>VLOOKUP(A12,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2148,13 +2092,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I13" t="str">
         <f>VLOOKUP(A13,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2163,13 +2107,13 @@
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I14" t="str">
         <f>VLOOKUP(A14,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2178,41 +2122,41 @@
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I15" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I16" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I17" t="str">
         <f>VLOOKUP(A17,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2221,13 +2165,13 @@
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I18" t="str">
         <f>VLOOKUP(A18,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2236,13 +2180,13 @@
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I19" t="str">
         <f>VLOOKUP(A19,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2251,13 +2195,13 @@
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I20" t="str">
         <f>VLOOKUP(A20,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2266,13 +2210,13 @@
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I21" t="str">
         <f>VLOOKUP(A21,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2281,13 +2225,13 @@
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I22" t="str">
         <f>VLOOKUP(A22,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2296,13 +2240,13 @@
     </row>
     <row r="23" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I23" t="str">
         <f>VLOOKUP(A23,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2311,13 +2255,13 @@
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I24" t="str">
         <f>VLOOKUP(A24,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2326,13 +2270,13 @@
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I25" t="str">
         <f>VLOOKUP(A25,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2341,13 +2285,13 @@
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I26" t="str">
         <f>VLOOKUP(A26,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2356,13 +2300,13 @@
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D27" s="7"/>
       <c r="I27" t="str">
@@ -2372,13 +2316,13 @@
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I28" t="str">
         <f>VLOOKUP(A28,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2387,13 +2331,13 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I29" t="str">
         <f>VLOOKUP(A29,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2402,13 +2346,13 @@
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I30" t="str">
         <f>VLOOKUP(A30,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2417,13 +2361,13 @@
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I31" t="str">
         <f>VLOOKUP(A31,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2432,13 +2376,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I32" t="str">
         <f>VLOOKUP(A32,'[1]Controle de conferencia LOA'!A$2:I$47,9,FALSE)</f>
@@ -2447,206 +2391,206 @@
     </row>
     <row r="33" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I35" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I37" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I38" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I39" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I40" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I41" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="I42" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="I43" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="I44" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="I45" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="I46" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="I47" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="I48" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="I49" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="I50" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>